<commit_message>
Added 2018 NFL Divisional Round Forecasts
</commit_message>
<xml_diff>
--- a/NFL2018/Weekly Forecasts/WeekWCMatrix.xlsx
+++ b/NFL2018/Weekly Forecasts/WeekWCMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MerrerPredictifier\MerrerPredictifier\NFL2018\Weekly Forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FB1BB855-E23A-44AE-964B-BC8D539AFC20}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3B25837F-41A1-4E13-9636-33EBE3734F78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projected Bracket" sheetId="15" r:id="rId1"/>
@@ -714,30 +714,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -850,6 +826,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1198,7 +1198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF079E1-9A36-40FA-8D19-B1CA7FE6E88D}">
   <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
@@ -1215,388 +1215,388 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="49"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="21" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="44"/>
     </row>
     <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="50"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="23" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="24"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="44"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="25" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="52"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="44"/>
     </row>
     <row r="6" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="27" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="52"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="44"/>
     </row>
     <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="52"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="44"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="50"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="29" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="44"/>
     </row>
     <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="55">
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="47">
         <v>33.44763011047398</v>
       </c>
-      <c r="I9" s="56">
+      <c r="I9" s="48">
         <v>33.74761805047639</v>
       </c>
-      <c r="J9" s="57"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="52"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="44"/>
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="50"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="52"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="44"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="29" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="32" t="s">
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="33" t="s">
+      <c r="K11" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="52"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="44"/>
     </row>
     <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="60">
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="52">
         <v>33.118672976265408</v>
       </c>
-      <c r="G12" s="61">
+      <c r="G12" s="53">
         <v>29.89880922023816</v>
       </c>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="60">
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="52">
         <v>32.122963375407323</v>
       </c>
-      <c r="K12" s="61">
+      <c r="K12" s="53">
         <v>30.738005652398869</v>
       </c>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="52"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="44"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="52"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="44"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B14" s="50"/>
-      <c r="C14" s="34" t="s">
+      <c r="B14" s="42"/>
+      <c r="C14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="51"/>
-      <c r="F14" s="29" t="s">
+      <c r="E14" s="43"/>
+      <c r="F14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="32" t="s">
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="37" t="s">
+      <c r="K14" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="51"/>
-      <c r="M14" s="38" t="s">
+      <c r="L14" s="43"/>
+      <c r="M14" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="39" t="s">
+      <c r="N14" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="O14" s="52"/>
+      <c r="O14" s="44"/>
     </row>
     <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="50"/>
-      <c r="C15" s="60">
+      <c r="B15" s="42"/>
+      <c r="C15" s="52">
         <v>25.794986841002629</v>
       </c>
-      <c r="D15" s="61">
+      <c r="D15" s="53">
         <v>23.20145295970941</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="60">
+      <c r="E15" s="43"/>
+      <c r="F15" s="52">
         <v>29.557663688467262</v>
       </c>
-      <c r="G15" s="61">
+      <c r="G15" s="53">
         <v>26.121879375624129</v>
       </c>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="60">
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="52">
         <v>29.761215047756991</v>
       </c>
-      <c r="K15" s="61">
+      <c r="K15" s="53">
         <v>24.501025299794939</v>
       </c>
-      <c r="L15" s="51"/>
-      <c r="M15" s="60">
+      <c r="L15" s="43"/>
+      <c r="M15" s="52">
         <v>27.389939922012019</v>
       </c>
-      <c r="N15" s="61">
+      <c r="N15" s="53">
         <v>26.340862131827571</v>
       </c>
-      <c r="O15" s="52"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="52"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="44"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B17" s="50"/>
-      <c r="C17" s="40" t="s">
+      <c r="B17" s="42"/>
+      <c r="C17" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="51"/>
-      <c r="F17" s="42" t="s">
+      <c r="E17" s="43"/>
+      <c r="F17" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="43" t="s">
+      <c r="G17" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="44" t="s">
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="37" t="s">
+      <c r="K17" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="L17" s="51"/>
-      <c r="M17" s="45" t="s">
+      <c r="L17" s="43"/>
+      <c r="M17" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="46" t="s">
+      <c r="N17" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O17" s="52"/>
+      <c r="O17" s="44"/>
     </row>
     <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="50"/>
-      <c r="C18" s="60">
+      <c r="B18" s="42"/>
+      <c r="C18" s="52">
         <v>25.4928525014295</v>
       </c>
-      <c r="D18" s="61">
+      <c r="D18" s="53">
         <v>24.674574265085148</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="60">
+      <c r="E18" s="43"/>
+      <c r="F18" s="52">
         <v>21.163259367348129</v>
       </c>
-      <c r="G18" s="61">
+      <c r="G18" s="53">
         <v>20.244260151147969</v>
       </c>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="62">
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="54">
         <v>20.697602660479468</v>
       </c>
-      <c r="K18" s="63">
+      <c r="K18" s="55">
         <v>23.26179834764033</v>
       </c>
-      <c r="L18" s="51"/>
-      <c r="M18" s="60">
+      <c r="L18" s="43"/>
+      <c r="M18" s="52">
         <v>24.552015089596981</v>
       </c>
-      <c r="N18" s="61">
+      <c r="N18" s="53">
         <v>18.013821997235599</v>
       </c>
-      <c r="O18" s="52"/>
+      <c r="O18" s="44"/>
     </row>
     <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="66"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5237,8 +5237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1D648B-F383-4192-B0B7-E082D9482495}">
   <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6561,7 +6561,7 @@
         <v>40</v>
       </c>
       <c r="B32" s="20">
-        <f>VLOOKUP(A32, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" ref="B32:B43" si="19">VLOOKUP(A32, $A$17:$C$28, 3, FALSE)</f>
         <v>0.19859312841608465</v>
       </c>
     </row>
@@ -6570,7 +6570,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="20">
-        <f>VLOOKUP(A33, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>0.17988017664664599</v>
       </c>
     </row>
@@ -6579,7 +6579,7 @@
         <v>41</v>
       </c>
       <c r="B34" s="20">
-        <f>VLOOKUP(A34, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>0.15457721603587604</v>
       </c>
     </row>
@@ -6588,7 +6588,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="20">
-        <f>VLOOKUP(A35, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>0.12967392167873126</v>
       </c>
     </row>
@@ -6597,7 +6597,7 @@
         <v>42</v>
       </c>
       <c r="B36" s="20">
-        <f>VLOOKUP(A36, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>8.2688781674881764E-2</v>
       </c>
     </row>
@@ -6606,7 +6606,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="20">
-        <f>VLOOKUP(A37, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>5.2555504523340568E-2</v>
       </c>
     </row>
@@ -6615,7 +6615,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="20">
-        <f>VLOOKUP(A38, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>4.5294340159978075E-2</v>
       </c>
     </row>
@@ -6624,7 +6624,7 @@
         <v>44</v>
       </c>
       <c r="B39" s="20">
-        <f>VLOOKUP(A39, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>4.2125429722208604E-2</v>
       </c>
     </row>
@@ -6633,7 +6633,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="20">
-        <f>VLOOKUP(A40, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>4.1976462328220811E-2</v>
       </c>
     </row>
@@ -6642,7 +6642,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="20">
-        <f>VLOOKUP(A41, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>3.8642430432490042E-2</v>
       </c>
     </row>
@@ -6651,7 +6651,7 @@
         <v>43</v>
       </c>
       <c r="B42" s="20">
-        <f>VLOOKUP(A42, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>1.8100687471342261E-2</v>
       </c>
     </row>
@@ -6660,7 +6660,7 @@
         <v>45</v>
       </c>
       <c r="B43" s="20">
-        <f>VLOOKUP(A43, $A$17:$C$28, 3, FALSE)</f>
+        <f t="shared" si="19"/>
         <v>1.5891920910199857E-2</v>
       </c>
     </row>

</xml_diff>